<commit_message>
Updated release doc folder
</commit_message>
<xml_diff>
--- a/src/Pickles/MIL_pickles/Output/AN210/AN210_TestScript_Desktop_Analysis_Validation_UR.xlsx
+++ b/src/Pickles/MIL_pickles/Output/AN210/AN210_TestScript_Desktop_Analysis_Validation_UR.xlsx
@@ -18,12 +18,14 @@
     <x:sheet name="DRAGANDDROPIMPORT" sheetId="11" r:id="rId11"/>
     <x:sheet name="ENABLEDENTINE" sheetId="12" r:id="rId12"/>
     <x:sheet name="IMAGEEXPORT" sheetId="13" r:id="rId13"/>
-    <x:sheet name="MAGNIFYIMAGE" sheetId="14" r:id="rId14"/>
-    <x:sheet name="RADIOGRAPHQUALITYGRADING" sheetId="15" r:id="rId15"/>
-    <x:sheet name="REPOSITIONCARIESROI" sheetId="16" r:id="rId16"/>
-    <x:sheet name="SHOWPROGRESS" sheetId="17" r:id="rId17"/>
-    <x:sheet name="TEXTREPORTEXPORT" sheetId="18" r:id="rId18"/>
-    <x:sheet name="TOGGLEANNOTATIONVISIBILITY" sheetId="19" r:id="rId19"/>
+    <x:sheet name="IMAGEID" sheetId="14" r:id="rId14"/>
+    <x:sheet name="MAGNIFYIMAGE" sheetId="15" r:id="rId15"/>
+    <x:sheet name="RADIOGRAPHQUALITYGRADING" sheetId="16" r:id="rId16"/>
+    <x:sheet name="REPOSITIONCARIESROI" sheetId="17" r:id="rId17"/>
+    <x:sheet name="SHOWPROGRESS" sheetId="18" r:id="rId18"/>
+    <x:sheet name="SUBMITIMAGES" sheetId="19" r:id="rId19"/>
+    <x:sheet name="TEXTREPORTEXPORT" sheetId="20" r:id="rId20"/>
+    <x:sheet name="TOGGLEANNOTATIONVISIBILITY" sheetId="21" r:id="rId21"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="237">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="268">
   <x:si>
     <x:t>AddCariesROI</x:t>
   </x:si>
@@ -496,6 +498,37 @@
     <x:t>the post-export command is executed</x:t>
   </x:si>
   <x:si>
+    <x:t>ImageID</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@UR, @UR023, @Analysis</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">	As a user
+	I want to be able to see the filename name next to the image
+	And be able to edit that ID to whatever text I wish
+	So that I can identify and label any of the images on the analysis page
+    And confirm that I submitted the correct image for analysis</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ShowImageIDAsFilename</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@UR023-1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I have submitted an image for analysis</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the image is displayed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the ID of the image is shown</x:t>
+  </x:si>
+  <x:si>
+    <x:t>set as the image filename</x:t>
+  </x:si>
+  <x:si>
     <x:t>MagnifyImage</x:t>
   </x:si>
   <x:si>
@@ -540,7 +573,7 @@
     <x:t>RadiographQualityGrading</x:t>
   </x:si>
   <x:si>
-    <x:t>@UR, @UR040, @DesktopOnly, @Analysis</x:t>
+    <x:t>@UR, @UR040, @Analysis</x:t>
   </x:si>
   <x:si>
     <x:t>As a dentist
@@ -702,10 +735,78 @@
     <x:t>the analysis status is reported at relevant stages</x:t>
   </x:si>
   <x:si>
+    <x:t>SubmitImages</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@UR, @UR016, @Analysis</x:t>
+  </x:si>
+  <x:si>
+    <x:t>As a dentist
+I want to submit one or more images for analysis
+So that I can request caries detection on my patients' images</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SubmitSingleImage</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@UR016-1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I am authorized with analysis permissions</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I navigate to the Analysis page</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I browse for a single bitewing image</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the image is sent</x:t>
+  </x:si>
+  <x:si>
+    <x:t>results are displayed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SubmitMultipleImages</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@UR016-2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I browse and select 2 bitewing images</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the images are sent</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the images are displayed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>results for both images are displayed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SubmitTiffImage</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@UR016-3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I browse for a single tiff bitewing image</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SubmitDICOMImage</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@UR016-4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I browse for a single DICOM bitewing image</x:t>
+  </x:si>
+  <x:si>
     <x:t>TextReportExport</x:t>
   </x:si>
   <x:si>
-    <x:t>@UR, @UR039, @DesktopOnly, @Analysis</x:t>
+    <x:t>@UR, @UR039, @Analysis</x:t>
   </x:si>
   <x:si>
     <x:t>As a dentist
@@ -1178,7 +1279,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B18"/>
+  <x:dimension ref="A1:B20"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -1186,7 +1287,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:2">
       <x:c r="A1" s="1" t="s">
-        <x:v>236</x:v>
+        <x:v>267</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:2">
@@ -1251,27 +1352,37 @@
     </x:row>
     <x:row r="14" spans="1:2">
       <x:c r="B14" s="4" t="s">
-        <x:v>160</x:v>
+        <x:v>156</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:2">
       <x:c r="B15" s="4" t="s">
-        <x:v>184</x:v>
+        <x:v>169</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:2">
       <x:c r="B16" s="4" t="s">
-        <x:v>206</x:v>
+        <x:v>193</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:2">
       <x:c r="B17" s="4" t="s">
-        <x:v>213</x:v>
+        <x:v>215</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:2">
       <x:c r="B18" s="4" t="s">
-        <x:v>224</x:v>
+        <x:v>222</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:2">
+      <x:c r="B19" s="4" t="s">
+        <x:v>244</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:2">
+      <x:c r="B20" s="4" t="s">
+        <x:v>255</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1287,12 +1398,14 @@
     <x:hyperlink ref="B10" location="'DRAGANDDROPIMPORT'!A1" display="DragAndDropImport"/>
     <x:hyperlink ref="B11" location="'ENABLEDENTINE'!A1" display="EnableDentine"/>
     <x:hyperlink ref="B12" location="'IMAGEEXPORT'!A1" display="ImageExport"/>
-    <x:hyperlink ref="B13" location="'MAGNIFYIMAGE'!A1" display="MagnifyImage"/>
-    <x:hyperlink ref="B14" location="'RADIOGRAPHQUALITYGRADING'!A1" display="RadiographQualityGrading"/>
-    <x:hyperlink ref="B15" location="'REPOSITIONCARIESROI'!A1" display="RepositionCariesROI"/>
-    <x:hyperlink ref="B16" location="'SHOWPROGRESS'!A1" display="ShowProgress"/>
-    <x:hyperlink ref="B17" location="'TEXTREPORTEXPORT'!A1" display="TextReportExport"/>
-    <x:hyperlink ref="B18" location="'TOGGLEANNOTATIONVISIBILITY'!A1" display="ToggleAnnotationVisibility"/>
+    <x:hyperlink ref="B13" location="'IMAGEID'!A1" display="ImageID"/>
+    <x:hyperlink ref="B14" location="'MAGNIFYIMAGE'!A1" display="MagnifyImage"/>
+    <x:hyperlink ref="B15" location="'RADIOGRAPHQUALITYGRADING'!A1" display="RadiographQualityGrading"/>
+    <x:hyperlink ref="B16" location="'REPOSITIONCARIESROI'!A1" display="RepositionCariesROI"/>
+    <x:hyperlink ref="B17" location="'SHOWPROGRESS'!A1" display="ShowProgress"/>
+    <x:hyperlink ref="B18" location="'SUBMITIMAGES'!A1" display="SubmitImages"/>
+    <x:hyperlink ref="B19" location="'TEXTREPORTEXPORT'!A1" display="TextReportExport"/>
+    <x:hyperlink ref="B20" location="'TOGGLEANNOTATIONVISIBILITY'!A1" display="ToggleAnnotationVisibility"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1307,7 +1420,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D9"/>
+  <x:dimension ref="A1:D38"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -1315,7 +1428,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>206</x:v>
+        <x:v>193</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
@@ -1323,17 +1436,17 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>207</x:v>
+        <x:v>194</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4">
       <x:c r="B3" s="0" t="s">
-        <x:v>208</x:v>
+        <x:v>195</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
       <x:c r="B5" s="1" t="s">
-        <x:v>209</x:v>
+        <x:v>196</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4">
@@ -1341,24 +1454,220 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C6" s="2" t="s">
-        <x:v>210</x:v>
+        <x:v>197</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4"/>
     <x:row r="8" spans="1:4">
       <x:c r="C8" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>211</x:v>
+        <x:v>198</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4">
       <x:c r="C9" s="3" t="s">
-        <x:v>9</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
+        <x:v>199</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:4">
+      <x:c r="C10" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>200</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:4">
+      <x:c r="C11" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>201</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:4">
+      <x:c r="C12" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>202</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:4">
+      <x:c r="C13" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>203</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:4">
+      <x:c r="C14" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>204</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:4">
+      <x:c r="C15" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>205</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:4">
+      <x:c r="B17" s="1" t="s">
+        <x:v>206</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:4">
+      <x:c r="B18" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C18" s="2" t="s">
+        <x:v>207</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:4"/>
+    <x:row r="20" spans="1:4">
+      <x:c r="C20" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:4">
+      <x:c r="C21" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:4">
+      <x:c r="C22" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:4">
+      <x:c r="C23" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>208</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:4">
+      <x:c r="C24" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="s">
+        <x:v>209</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:4">
+      <x:c r="C25" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D25" s="0" t="s">
+        <x:v>204</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:4">
+      <x:c r="C26" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D26" s="0" t="s">
+        <x:v>205</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:4">
+      <x:c r="B28" s="1" t="s">
+        <x:v>210</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:4">
+      <x:c r="B29" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C29" s="2" t="s">
+        <x:v>211</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:4"/>
+    <x:row r="31" spans="1:4">
+      <x:c r="C31" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:4">
+      <x:c r="C32" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D32" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:4">
+      <x:c r="C33" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="s">
         <x:v>212</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:4">
+      <x:c r="C34" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D34" s="0" t="s">
+        <x:v>213</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:4">
+      <x:c r="C35" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D35" s="0" t="s">
+        <x:v>214</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:4">
+      <x:c r="C36" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D36" s="0" t="s">
+        <x:v>203</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:4">
+      <x:c r="C37" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D37" s="0" t="s">
+        <x:v>204</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:4">
+      <x:c r="C38" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D38" s="0" t="s">
+        <x:v>205</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1375,7 +1684,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D22"/>
+  <x:dimension ref="A1:D9"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -1383,7 +1692,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>213</x:v>
+        <x:v>215</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
@@ -1391,17 +1700,17 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>214</x:v>
+        <x:v>216</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4">
       <x:c r="B3" s="0" t="s">
-        <x:v>215</x:v>
+        <x:v>217</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
       <x:c r="B5" s="1" t="s">
-        <x:v>216</x:v>
+        <x:v>218</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4">
@@ -1409,110 +1718,24 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C6" s="2" t="s">
-        <x:v>217</x:v>
+        <x:v>219</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4"/>
     <x:row r="8" spans="1:4">
       <x:c r="C8" s="3" t="s">
-        <x:v>5</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>130</x:v>
+        <x:v>220</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4">
       <x:c r="C9" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>131</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:4">
-      <x:c r="C10" s="3" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D10" s="0" t="s">
-        <x:v>218</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:4">
-      <x:c r="C11" s="3" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D11" s="0" t="s">
-        <x:v>219</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:4">
-      <x:c r="C12" s="3" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D12" s="0" t="s">
-        <x:v>220</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:4">
-      <x:c r="B14" s="1" t="s">
         <x:v>221</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:4">
-      <x:c r="B15" s="2" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C15" s="2" t="s">
-        <x:v>222</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:4"/>
-    <x:row r="17" spans="1:4">
-      <x:c r="C17" s="3" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D17" s="0" t="s">
-        <x:v>130</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:4">
-      <x:c r="C18" s="3" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D18" s="0" t="s">
-        <x:v>136</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:4">
-      <x:c r="C19" s="3" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D19" s="0" t="s">
-        <x:v>137</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:4">
-      <x:c r="C20" s="3" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D20" s="0" t="s">
-        <x:v>223</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:4">
-      <x:c r="C21" s="3" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D21" s="0" t="s">
-        <x:v>219</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="22" spans="1:4">
-      <x:c r="C22" s="3" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D22" s="0" t="s">
-        <x:v>220</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1529,6 +1752,446 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
+  <x:dimension ref="A1:D43"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:4">
+      <x:c r="A1" s="1" t="s">
+        <x:v>222</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:4">
+      <x:c r="B2" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C2" s="2" t="s">
+        <x:v>223</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:4">
+      <x:c r="B3" s="0" t="s">
+        <x:v>224</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:4">
+      <x:c r="B5" s="1" t="s">
+        <x:v>225</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:4">
+      <x:c r="B6" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C6" s="2" t="s">
+        <x:v>226</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:4"/>
+    <x:row r="8" spans="1:4">
+      <x:c r="C8" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>227</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:4">
+      <x:c r="C9" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>228</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:4">
+      <x:c r="C10" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>229</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:4">
+      <x:c r="C11" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>230</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:4">
+      <x:c r="C12" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>153</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:4">
+      <x:c r="C13" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>231</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:4">
+      <x:c r="B15" s="1" t="s">
+        <x:v>232</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:4">
+      <x:c r="B16" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C16" s="2" t="s">
+        <x:v>233</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:4"/>
+    <x:row r="18" spans="1:4">
+      <x:c r="C18" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>227</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:4">
+      <x:c r="C19" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>228</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:4">
+      <x:c r="C20" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>234</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:4">
+      <x:c r="C21" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>235</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:4">
+      <x:c r="C22" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>236</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:4">
+      <x:c r="C23" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>237</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:4">
+      <x:c r="B25" s="1" t="s">
+        <x:v>238</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:4">
+      <x:c r="B26" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C26" s="2" t="s">
+        <x:v>239</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:4"/>
+    <x:row r="28" spans="1:4">
+      <x:c r="C28" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="s">
+        <x:v>227</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:4">
+      <x:c r="C29" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="s">
+        <x:v>228</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:4">
+      <x:c r="C30" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="s">
+        <x:v>240</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:4">
+      <x:c r="C31" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>230</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:4">
+      <x:c r="C32" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D32" s="0" t="s">
+        <x:v>153</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:4">
+      <x:c r="C33" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="s">
+        <x:v>231</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:4">
+      <x:c r="B35" s="1" t="s">
+        <x:v>241</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:4">
+      <x:c r="B36" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C36" s="2" t="s">
+        <x:v>242</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:4"/>
+    <x:row r="38" spans="1:4">
+      <x:c r="C38" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D38" s="0" t="s">
+        <x:v>227</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:4">
+      <x:c r="C39" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D39" s="0" t="s">
+        <x:v>228</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:4">
+      <x:c r="C40" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D40" s="0" t="s">
+        <x:v>243</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:4">
+      <x:c r="C41" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D41" s="0" t="s">
+        <x:v>230</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:4">
+      <x:c r="C42" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D42" s="0" t="s">
+        <x:v>153</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:4">
+      <x:c r="C43" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D43" s="0" t="s">
+        <x:v>231</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:D22"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:4">
+      <x:c r="A1" s="1" t="s">
+        <x:v>244</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:4">
+      <x:c r="B2" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C2" s="2" t="s">
+        <x:v>245</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:4">
+      <x:c r="B3" s="0" t="s">
+        <x:v>246</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:4">
+      <x:c r="B5" s="1" t="s">
+        <x:v>247</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:4">
+      <x:c r="B6" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C6" s="2" t="s">
+        <x:v>248</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:4"/>
+    <x:row r="8" spans="1:4">
+      <x:c r="C8" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>130</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:4">
+      <x:c r="C9" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>131</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:4">
+      <x:c r="C10" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>249</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:4">
+      <x:c r="C11" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>250</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:4">
+      <x:c r="C12" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>251</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:4">
+      <x:c r="B14" s="1" t="s">
+        <x:v>252</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:4">
+      <x:c r="B15" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C15" s="2" t="s">
+        <x:v>253</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:4"/>
+    <x:row r="17" spans="1:4">
+      <x:c r="C17" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>130</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:4">
+      <x:c r="C18" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>136</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:4">
+      <x:c r="C19" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>137</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:4">
+      <x:c r="C20" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>254</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:4">
+      <x:c r="C21" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>250</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:4">
+      <x:c r="C22" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>251</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
   <x:dimension ref="A1:D20"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
@@ -1537,7 +2200,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>224</x:v>
+        <x:v>255</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
@@ -1545,17 +2208,17 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>225</x:v>
+        <x:v>256</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4">
       <x:c r="B3" s="0" t="s">
-        <x:v>226</x:v>
+        <x:v>257</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
       <x:c r="B5" s="1" t="s">
-        <x:v>227</x:v>
+        <x:v>258</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4">
@@ -1563,7 +2226,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C6" s="2" t="s">
-        <x:v>228</x:v>
+        <x:v>259</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4"/>
@@ -1588,7 +2251,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>229</x:v>
+        <x:v>260</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:4">
@@ -1596,12 +2259,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>230</x:v>
+        <x:v>261</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:4">
       <x:c r="B13" s="1" t="s">
-        <x:v>231</x:v>
+        <x:v>262</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4">
@@ -1609,7 +2272,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C14" s="2" t="s">
-        <x:v>232</x:v>
+        <x:v>263</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:4"/>
@@ -1634,7 +2297,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>233</x:v>
+        <x:v>264</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:4">
@@ -1642,7 +2305,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>234</x:v>
+        <x:v>265</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:4">
@@ -1650,7 +2313,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>235</x:v>
+        <x:v>266</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -3185,7 +3848,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D21"/>
+  <x:dimension ref="A1:D11"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -3228,93 +3891,31 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>152</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4">
       <x:c r="C9" s="3" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>153</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:4">
       <x:c r="C10" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>152</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:4">
       <x:c r="C11" s="3" t="s">
-        <x:v>9</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>153</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:4">
-      <x:c r="B13" s="1" t="s">
-        <x:v>154</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:4">
-      <x:c r="B14" s="2" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C14" s="2" t="s">
         <x:v>155</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:4"/>
-    <x:row r="16" spans="1:4">
-      <x:c r="C16" s="3" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D16" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:4">
-      <x:c r="C17" s="3" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D17" s="0" t="s">
-        <x:v>156</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:4">
-      <x:c r="C18" s="3" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D18" s="0" t="s">
-        <x:v>157</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:4">
-      <x:c r="C19" s="3" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D19" s="0" t="s">
-        <x:v>158</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:4">
-      <x:c r="C20" s="3" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D20" s="0" t="s">
-        <x:v>159</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:4">
-      <x:c r="C21" s="3" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D21" s="0" t="s">
-        <x:v>158</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -3331,7 +3932,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D38"/>
+  <x:dimension ref="A1:D21"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -3339,7 +3940,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>160</x:v>
+        <x:v>156</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
@@ -3347,17 +3948,17 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>161</x:v>
+        <x:v>157</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4">
       <x:c r="B3" s="0" t="s">
-        <x:v>162</x:v>
+        <x:v>158</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
       <x:c r="B5" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4">
@@ -3365,7 +3966,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C6" s="2" t="s">
-        <x:v>164</x:v>
+        <x:v>160</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4"/>
@@ -3374,58 +3975,58 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>165</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4">
       <x:c r="C9" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>166</x:v>
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:4">
       <x:c r="C10" s="3" t="s">
-        <x:v>9</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>167</x:v>
+        <x:v>161</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:4">
       <x:c r="C11" s="3" t="s">
-        <x:v>11</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>168</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:4">
-      <x:c r="C12" s="3" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D12" s="0" t="s">
-        <x:v>169</x:v>
+        <x:v>162</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:4">
+      <x:c r="B13" s="1" t="s">
+        <x:v>163</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4">
-      <x:c r="B14" s="1" t="s">
-        <x:v>170</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:4">
-      <x:c r="B15" s="2" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C15" s="2" t="s">
-        <x:v>171</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:4"/>
+      <x:c r="B14" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C14" s="2" t="s">
+        <x:v>164</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:4"/>
+    <x:row r="16" spans="1:4">
+      <x:c r="C16" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
     <x:row r="17" spans="1:4">
       <x:c r="C17" s="3" t="s">
-        <x:v>5</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
         <x:v>165</x:v>
@@ -3444,123 +4045,23 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>172</x:v>
+        <x:v>167</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:4">
       <x:c r="C20" s="3" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>173</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="22" spans="1:4">
-      <x:c r="B22" s="1" t="s">
-        <x:v>174</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="23" spans="1:4">
-      <x:c r="B23" s="2" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C23" s="2" t="s">
-        <x:v>175</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="24" spans="1:4"/>
-    <x:row r="25" spans="1:4">
-      <x:c r="C25" s="3" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D25" s="0" t="s">
-        <x:v>165</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="26" spans="1:4">
-      <x:c r="C26" s="3" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D26" s="0" t="s">
-        <x:v>166</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="27" spans="1:4">
-      <x:c r="C27" s="3" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D27" s="0" t="s">
-        <x:v>176</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="28" spans="1:4">
-      <x:c r="C28" s="3" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D28" s="0" t="s">
-        <x:v>177</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="29" spans="1:4">
-      <x:c r="C29" s="3" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D29" s="0" t="s">
-        <x:v>178</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="31" spans="1:4">
-      <x:c r="B31" s="1" t="s">
-        <x:v>179</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="32" spans="1:4">
-      <x:c r="B32" s="2" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C32" s="2" t="s">
-        <x:v>180</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="33" spans="1:4"/>
-    <x:row r="34" spans="1:4">
-      <x:c r="C34" s="3" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D34" s="0" t="s">
-        <x:v>165</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="35" spans="1:4">
-      <x:c r="C35" s="3" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D35" s="0" t="s">
-        <x:v>166</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="36" spans="1:4">
-      <x:c r="C36" s="3" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D36" s="0" t="s">
-        <x:v>181</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="37" spans="1:4">
-      <x:c r="C37" s="3" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D37" s="0" t="s">
-        <x:v>182</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="38" spans="1:4">
-      <x:c r="C38" s="3" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D38" s="0" t="s">
-        <x:v>183</x:v>
+        <x:v>168</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:4">
+      <x:c r="C21" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>167</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -3585,7 +4086,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>184</x:v>
+        <x:v>169</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
@@ -3593,17 +4094,17 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>185</x:v>
+        <x:v>170</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4">
       <x:c r="B3" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>171</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
       <x:c r="B5" s="1" t="s">
-        <x:v>187</x:v>
+        <x:v>172</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4">
@@ -3611,7 +4112,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C6" s="2" t="s">
-        <x:v>188</x:v>
+        <x:v>173</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4"/>
@@ -3620,31 +4121,31 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>189</x:v>
+        <x:v>174</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4">
       <x:c r="C9" s="3" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>190</x:v>
+        <x:v>175</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:4">
       <x:c r="C10" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>191</x:v>
+        <x:v>176</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:4">
       <x:c r="C11" s="3" t="s">
-        <x:v>9</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>192</x:v>
+        <x:v>177</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:4">
@@ -3652,163 +4153,145 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>193</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:4">
-      <x:c r="C13" s="3" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D13" s="0" t="s">
-        <x:v>194</x:v>
+        <x:v>178</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4">
-      <x:c r="C14" s="3" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D14" s="0" t="s">
-        <x:v>195</x:v>
+      <x:c r="B14" s="1" t="s">
+        <x:v>179</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:4">
-      <x:c r="C15" s="3" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D15" s="0" t="s">
-        <x:v>196</x:v>
-      </x:c>
-    </x:row>
+      <x:c r="B15" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C15" s="2" t="s">
+        <x:v>180</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:4"/>
     <x:row r="17" spans="1:4">
-      <x:c r="B17" s="1" t="s">
-        <x:v>197</x:v>
+      <x:c r="C17" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>174</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:4">
-      <x:c r="B18" s="2" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C18" s="2" t="s">
-        <x:v>198</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:4"/>
+      <x:c r="C18" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>175</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:4">
+      <x:c r="C19" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>181</x:v>
+      </x:c>
+    </x:row>
     <x:row r="20" spans="1:4">
       <x:c r="C20" s="3" t="s">
-        <x:v>5</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:4">
-      <x:c r="C21" s="3" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D21" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>182</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:4">
-      <x:c r="C22" s="3" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D22" s="0" t="s">
-        <x:v>20</x:v>
+      <x:c r="B22" s="1" t="s">
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:4">
-      <x:c r="C23" s="3" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D23" s="0" t="s">
-        <x:v>199</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="24" spans="1:4">
-      <x:c r="C24" s="3" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D24" s="0" t="s">
-        <x:v>200</x:v>
-      </x:c>
-    </x:row>
+      <x:c r="B23" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C23" s="2" t="s">
+        <x:v>184</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:4"/>
     <x:row r="25" spans="1:4">
       <x:c r="C25" s="3" t="s">
-        <x:v>11</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="D25" s="0" t="s">
-        <x:v>195</x:v>
+        <x:v>174</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:4">
       <x:c r="C26" s="3" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D26" s="0" t="s">
-        <x:v>196</x:v>
+        <x:v>175</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:4">
+      <x:c r="C27" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="s">
+        <x:v>185</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:4">
-      <x:c r="B28" s="1" t="s">
-        <x:v>201</x:v>
+      <x:c r="C28" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="s">
+        <x:v>186</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:4">
-      <x:c r="B29" s="2" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C29" s="2" t="s">
-        <x:v>202</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="30" spans="1:4"/>
+      <x:c r="C29" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="s">
+        <x:v>187</x:v>
+      </x:c>
+    </x:row>
     <x:row r="31" spans="1:4">
-      <x:c r="C31" s="3" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D31" s="0" t="s">
-        <x:v>6</x:v>
+      <x:c r="B31" s="1" t="s">
+        <x:v>188</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:4">
-      <x:c r="C32" s="3" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D32" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="33" spans="1:4">
-      <x:c r="C33" s="3" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D33" s="0" t="s">
-        <x:v>203</x:v>
-      </x:c>
-    </x:row>
+      <x:c r="B32" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C32" s="2" t="s">
+        <x:v>189</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:4"/>
     <x:row r="34" spans="1:4">
       <x:c r="C34" s="3" t="s">
-        <x:v>11</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="D34" s="0" t="s">
-        <x:v>204</x:v>
+        <x:v>174</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:4">
       <x:c r="C35" s="3" t="s">
-        <x:v>9</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D35" s="0" t="s">
-        <x:v>205</x:v>
+        <x:v>175</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:4">
       <x:c r="C36" s="3" t="s">
-        <x:v>11</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D36" s="0" t="s">
-        <x:v>194</x:v>
+        <x:v>190</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:4">
@@ -3816,7 +4299,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D37" s="0" t="s">
-        <x:v>195</x:v>
+        <x:v>191</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:4">
@@ -3824,7 +4307,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D38" s="0" t="s">
-        <x:v>196</x:v>
+        <x:v>192</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>